<commit_message>
Regione: REGIONE_CAMPANIA, Issuer: integrity:S1#VICAMPANIA
</commit_message>
<xml_diff>
--- a/REGIONE_CAMPANIA/integrity:S1#VICAMPANIA.xlsx
+++ b/REGIONE_CAMPANIA/integrity:S1#VICAMPANIA.xlsx
@@ -41,13 +41,13 @@
     <t>NGNVCN92S19L259C^^^&amp;2.16.840.1.113883.2.9.4.3.2&amp;ISO</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.a6824425c1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.4d02802ff5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721293636822</t>
+    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721298575810</t>
   </si>
   <si>
-    <t>18-07-2024:11:07:22</t>
+    <t>18-07-2024:12:29:39</t>
   </si>
 </sst>
 </file>

</xml_diff>